<commit_message>
Update of CAD, ASSEMBLY_INSTRUCTIONS and BOM
</commit_message>
<xml_diff>
--- a/BOM_proto.xlsx
+++ b/BOM_proto.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usherbrooke-my.sharepoint.com/personal/pelv2302_usherbrooke_ca/Documents/Session 4/Projet S4 (RoboAide)/3 Partie mécanique et électronique/3.1 Partie mécanique/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivi\Documents\UdeS\Session_4\Projet\projetS4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{9CA3E697-B04E-4AD8-B6C4-191F3B8B6C45}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{27184AA3-F059-4A88-9E92-3E4C42393D39}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C3B802-B4F4-433F-9EC6-7FC3AC2CC746}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="15196" xr2:uid="{4470428E-894C-4DAB-A980-78E8169B8C45}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$3:$F$3</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="61">
   <si>
     <t>Bill of material for the prototype</t>
   </si>
@@ -39,9 +42,6 @@
     <t>Vendor</t>
   </si>
   <si>
-    <t xml:space="preserve">Part number </t>
-  </si>
-  <si>
     <t>Servocity</t>
   </si>
   <si>
@@ -63,9 +63,6 @@
     <t>acryliq laser cut</t>
   </si>
   <si>
-    <t>3D printed</t>
-  </si>
-  <si>
     <t>vertical axel kit</t>
   </si>
   <si>
@@ -93,9 +90,6 @@
     <t>Amazon - BQLZR</t>
   </si>
   <si>
-    <t>Link</t>
-  </si>
-  <si>
     <t>https://www.amazon.ca/gp/product/B01K4MVXOU/ref=ppx_yo_dt_b_asin_title_o00_s00?ie=UTF8&amp;psc=1</t>
   </si>
   <si>
@@ -169,6 +163,60 @@
   </si>
   <si>
     <t>http://www.robotis.us/search.php?search_query=xm%20h%20430&amp;section=product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vendor part number </t>
+  </si>
+  <si>
+    <t>Assembly part number</t>
+  </si>
+  <si>
+    <t>Link to vendor's website</t>
+  </si>
+  <si>
+    <t>https://www.robotshop.com/en/cytron-12v-430rpm-15-57oz-gear-motor-encoder.html?fbclid=IwAR2z9R2E9fAauhUUTQctWkZS36Jk64Tj66HTLzBILs4lhKmntN9CRqr_dfk</t>
+  </si>
+  <si>
+    <t>RobotShop</t>
+  </si>
+  <si>
+    <t>DC Planetary Gearmotor</t>
+  </si>
+  <si>
+    <t>Cytron 12V, 430rpm, 15.57oz-in Gear Motor w / Encoder</t>
+  </si>
+  <si>
+    <t>Motor bracket</t>
+  </si>
+  <si>
+    <t>PLA 3D printed</t>
+  </si>
+  <si>
+    <t>Screw M3 x 30 mm</t>
+  </si>
+  <si>
+    <t>Nut M3</t>
+  </si>
+  <si>
+    <t>Nut #5-40</t>
+  </si>
+  <si>
+    <t>Screw #5-40, 3/4'' length</t>
+  </si>
+  <si>
+    <t>Screw #5-40, 1/2'' length</t>
+  </si>
+  <si>
+    <t>Screw #5-40, 3/8'' length</t>
+  </si>
+  <si>
+    <t>Motor shaft adaptator</t>
+  </si>
+  <si>
+    <t>Visit a hardware store</t>
+  </si>
+  <si>
+    <t>Hardware store</t>
   </si>
 </sst>
 </file>
@@ -249,7 +297,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -271,6 +319,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -587,312 +639,547 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C59EB11-D4FE-43B2-9AA6-00721766E975}">
-  <dimension ref="B2:F19"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:F19"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
+    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.19921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="88.53125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="140.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B2" s="3" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B4" s="2" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="6">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="6">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="E4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="6">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="6">
         <v>1</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="11">
+        <v>1</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="6">
+        <v>4</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="6">
         <v>2</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="D7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="5">
+        <v>634080</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="6">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="6">
+        <v>3</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="5">
+        <v>585454</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="6">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="6">
         <v>4</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="D9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="5">
+        <v>535130</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="6">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="6">
+        <v>3</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="5">
+        <v>585446</v>
+      </c>
+      <c r="F10" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B5" s="9" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="6">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="5">
+        <v>585416</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" s="6">
+        <v>9</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="6">
+        <v>6</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="5">
+        <v>585424</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" s="6">
+        <v>10</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="6">
+        <v>4</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="5">
+        <v>585468</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" s="6">
+        <v>11</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="6">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" s="6">
+        <v>12</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="6">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" s="6">
+        <v>13</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="6">
+        <v>2</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17" s="6">
+        <v>14</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="6">
+        <v>2</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18" s="6">
+        <v>15</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="5">
-        <v>634080</v>
-      </c>
-      <c r="E5" s="6">
-        <v>2</v>
-      </c>
-      <c r="F5" s="8" t="s">
+      <c r="C18" s="6">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19" s="6">
+        <v>16</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="6">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20" s="6">
+        <v>17</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="6">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A21" s="11">
+        <v>18</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="6">
+        <v>16</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A22" s="11">
+        <v>19</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="6">
+        <v>16</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23" s="6">
+        <v>20</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="6">
+        <v>16</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24" s="6">
+        <v>21</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="6">
+        <v>16</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25" s="6">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="5">
-        <v>585446</v>
-      </c>
-      <c r="E6" s="6">
-        <v>3</v>
-      </c>
-      <c r="F6" s="8" t="s">
+      <c r="B25" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" s="6">
+        <v>28</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A26" s="6">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="5">
-        <v>585416</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="8" t="s">
+      <c r="B26" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="6">
+        <v>60</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A27" s="11">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="5">
-        <v>585468</v>
-      </c>
-      <c r="E8" s="6">
+      <c r="B27" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="11">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F27" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="5">
-        <v>535130</v>
-      </c>
-      <c r="E9" s="6">
-        <v>4</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="5">
-        <v>585424</v>
-      </c>
-      <c r="E10" s="6">
-        <v>6</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="5">
-        <v>585454</v>
-      </c>
-      <c r="E11" s="6">
-        <v>3</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="6">
-        <v>3</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="6">
-        <v>1</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B14" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14" s="6">
-        <v>1</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B15" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E15" s="6">
-        <v>2</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E16" s="6">
-        <v>2</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B17" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E17" s="6">
-        <v>2</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B18" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E18" s="6">
-        <v>1</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B19" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E19" s="6">
-        <v>1</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
   </sheetData>
+  <autoFilter ref="A3:F3" xr:uid="{8563EF61-1E9F-4A95-9E31-C1B5B942B6B2}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:F20">
+      <sortCondition ref="F3"/>
+    </sortState>
+  </autoFilter>
   <hyperlinks>
-    <hyperlink ref="F13" r:id="rId1" xr:uid="{27D359DB-4CB4-4A74-8A1D-215091C46467}"/>
-    <hyperlink ref="F5" r:id="rId2" xr:uid="{AF6DD081-D890-4CFD-80FE-D99C9A135D63}"/>
-    <hyperlink ref="F6" r:id="rId3" xr:uid="{2E00DD2C-3EC3-4355-9411-5A62C971D199}"/>
-    <hyperlink ref="F7" r:id="rId4" xr:uid="{58500D27-EB04-48BA-8C42-1B2058A747E7}"/>
-    <hyperlink ref="F8" r:id="rId5" xr:uid="{2CD71D2C-814E-4B0A-B400-D4D27BA02A8B}"/>
+    <hyperlink ref="F5" r:id="rId1" xr:uid="{27D359DB-4CB4-4A74-8A1D-215091C46467}"/>
+    <hyperlink ref="F7" r:id="rId2" xr:uid="{AF6DD081-D890-4CFD-80FE-D99C9A135D63}"/>
+    <hyperlink ref="F10" r:id="rId3" xr:uid="{2E00DD2C-3EC3-4355-9411-5A62C971D199}"/>
+    <hyperlink ref="F11" r:id="rId4" xr:uid="{58500D27-EB04-48BA-8C42-1B2058A747E7}"/>
+    <hyperlink ref="F13" r:id="rId5" xr:uid="{2CD71D2C-814E-4B0A-B400-D4D27BA02A8B}"/>
     <hyperlink ref="F9" r:id="rId6" xr:uid="{35EB93BF-0449-48CA-8C6E-C9E53BF1A7A5}"/>
-    <hyperlink ref="F10" r:id="rId7" xr:uid="{DE043D1F-166E-4294-9330-4CF6CE4F08B1}"/>
-    <hyperlink ref="F11" r:id="rId8" xr:uid="{48982682-FC50-493A-9F4B-7AEA72856878}"/>
-    <hyperlink ref="F12" r:id="rId9" xr:uid="{D3C3A67B-3824-4499-A376-62ED47606BE5}"/>
+    <hyperlink ref="F12" r:id="rId7" xr:uid="{DE043D1F-166E-4294-9330-4CF6CE4F08B1}"/>
+    <hyperlink ref="F8" r:id="rId8" xr:uid="{48982682-FC50-493A-9F4B-7AEA72856878}"/>
+    <hyperlink ref="F4" r:id="rId9" xr:uid="{D3C3A67B-3824-4499-A376-62ED47606BE5}"/>
+    <hyperlink ref="F6" r:id="rId10" xr:uid="{76E0FF25-1194-4050-ADD0-32BBA240AC62}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId10"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId11"/>
 </worksheet>
 </file>
 

</xml_diff>